<commit_message>
Added comment for backstory generation
</commit_message>
<xml_diff>
--- a/Char_Info.xlsx
+++ b/Char_Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerwilson/Stuff/DND/AutoChar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F924C8BD-C4AD-684B-8C3E-A0AAAEF7F745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A271E2E0-F828-DB4A-9BE3-70824ED75ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{FF5BDC9C-1564-9842-ACA0-6308D30C81FE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{FF5BDC9C-1564-9842-ACA0-6308D30C81FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Armor" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Martial Weapons" sheetId="4" r:id="rId4"/>
     <sheet name="Player Backgrounds" sheetId="5" r:id="rId5"/>
     <sheet name="Player Subraces" sheetId="6" r:id="rId6"/>
+    <sheet name="Adjective" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="237">
   <si>
     <t>Name</t>
   </si>
@@ -705,6 +706,42 @@
   </si>
   <si>
     <t>0,0</t>
+  </si>
+  <si>
+    <t>Charming</t>
+  </si>
+  <si>
+    <t>Brutal</t>
+  </si>
+  <si>
+    <t>Tough</t>
+  </si>
+  <si>
+    <t>Sneaky</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Muscular</t>
+  </si>
+  <si>
+    <t>Caring</t>
+  </si>
+  <si>
+    <t>Apathetic</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Magical</t>
+  </si>
+  <si>
+    <t>Divine</t>
+  </si>
+  <si>
+    <t>Merciful</t>
   </si>
 </sst>
 </file>
@@ -2868,7 +2905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DF673C-25B6-FB4F-B7F9-5D08B1265B0C}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3173,4 +3210,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2816704-C24D-4C49-A9D2-24A8A3416261}">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>